<commit_message>
StopAll 5% wrong ans
</commit_message>
<xml_diff>
--- a/detalles_stopAll.xlsx
+++ b/detalles_stopAll.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francisco\Documents\01_ing\javaSolutions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Francisco\Documents\fr_docs\git\javaSolutions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A213DF1B-F380-4B21-BF11-D64343A8573E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6090" yWindow="435" windowWidth="19605" windowHeight="10920" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6090" yWindow="435" windowWidth="19605" windowHeight="10920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Macro1" sheetId="2" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>3 , 2</t>
   </si>
@@ -100,9 +99,6 @@
     <t>nombre 1</t>
   </si>
   <si>
-    <t xml:space="preserve">nombre 2 </t>
-  </si>
-  <si>
     <t xml:space="preserve">nombre 3 </t>
   </si>
   <si>
@@ -113,12 +109,21 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>output ex</t>
+  </si>
+  <si>
+    <t>My output</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -156,7 +161,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -195,9 +200,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -477,7 +482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64F09277-884A-4D4E-A5ED-E1DC920157B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -489,19 +494,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A2:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="5" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -697,7 +704,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>7</v>
       </c>
@@ -706,90 +713,137 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>8</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="C29" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -797,7 +851,10 @@
       <c r="A33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -805,7 +862,10 @@
       <c r="A34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>16</v>
       </c>
     </row>
@@ -813,7 +873,10 @@
       <c r="A35" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -821,58 +884,49 @@
       <c r="A36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="8" t="s">
         <v>15</v>
       </c>
+      <c r="C36" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="8" t="s">
+      <c r="B39" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>24</v>
       </c>
-      <c r="D39" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="B40">
-        <v>2</v>
-      </c>
-      <c r="C40">
-        <v>4</v>
-      </c>
-      <c r="D40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="B41">
         <v>8</v>
       </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
       <c r="D41">
         <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>28</v>
+      <c r="A42" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="B42">
         <v>2</v>
-      </c>
-      <c r="C42">
-        <v>3</v>
       </c>
       <c r="D42">
         <v>2</v>

</xml_diff>